<commit_message>
Ticket #9520 further corrections added to cal sheet by Steve Gaul.
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP03ISSM_00003.xlsx
+++ b/deployment/Omaha_Cal_Info_CP03ISSM_00003.xlsx
@@ -864,12 +864,6 @@
     <t>N00757</t>
   </si>
   <si>
-    <t>CP03ISSM-00003-SBD11-HYDGN</t>
-  </si>
-  <si>
-    <t>CP03ISSM-00003-SBD12-HYDGN</t>
-  </si>
-  <si>
     <t>R00024</t>
   </si>
   <si>
@@ -904,6 +898,12 @@
   </si>
   <si>
     <t>R00035</t>
+  </si>
+  <si>
+    <t>CP03ISSM-00003-HYDGN1</t>
+  </si>
+  <si>
+    <t>CP03ISSM-00003-HYDGN2</t>
   </si>
 </sst>
 </file>
@@ -2661,8 +2661,8 @@
   <dimension ref="A1:U365"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E185" sqref="E185:E190"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8"/>
@@ -2672,7 +2672,7 @@
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" style="4" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" style="43" customWidth="1"/>
-    <col min="6" max="6" width="16" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="33.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="62.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="7" customWidth="1"/>
@@ -2739,7 +2739,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="144" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F3" s="85">
         <v>11</v>
@@ -2766,10 +2766,10 @@
         <v>3</v>
       </c>
       <c r="E5" s="145" t="s">
-        <v>221</v>
-      </c>
-      <c r="F5" s="74" t="s">
-        <v>218</v>
+        <v>219</v>
+      </c>
+      <c r="F5" s="147" t="s">
+        <v>230</v>
       </c>
       <c r="I5" s="66" t="s">
         <v>138</v>
@@ -2789,10 +2789,10 @@
         <v>3</v>
       </c>
       <c r="E6" s="145" t="s">
-        <v>222</v>
-      </c>
-      <c r="F6" s="74" t="s">
-        <v>219</v>
+        <v>220</v>
+      </c>
+      <c r="F6" s="147" t="s">
+        <v>231</v>
       </c>
       <c r="I6" s="66" t="s">
         <v>138</v>
@@ -7087,7 +7087,7 @@
         <v>3</v>
       </c>
       <c r="E181" s="146" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F181" s="66" t="s">
         <v>183</v>
@@ -7110,7 +7110,7 @@
         <v>3</v>
       </c>
       <c r="E182" s="146" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F182" s="66" t="s">
         <v>184</v>
@@ -7133,7 +7133,7 @@
         <v>3</v>
       </c>
       <c r="E183" s="146" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F183" s="66" t="s">
         <v>185</v>
@@ -7166,7 +7166,7 @@
         <v>3</v>
       </c>
       <c r="E185" s="147" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F185" s="66" t="s">
         <v>186</v>
@@ -7203,7 +7203,7 @@
         <v>3</v>
       </c>
       <c r="E186" s="147" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F186" s="66" t="s">
         <v>187</v>
@@ -7240,7 +7240,7 @@
         <v>3</v>
       </c>
       <c r="E187" s="147" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F187" s="66" t="s">
         <v>188</v>
@@ -7277,7 +7277,7 @@
         <v>3</v>
       </c>
       <c r="E188" s="147" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F188" s="66" t="s">
         <v>189</v>
@@ -7314,7 +7314,7 @@
         <v>3</v>
       </c>
       <c r="E189" s="147" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F189" s="66" t="s">
         <v>190</v>
@@ -7351,7 +7351,7 @@
         <v>3</v>
       </c>
       <c r="E190" s="147" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F190" s="66" t="s">
         <v>191</v>

</xml_diff>